<commit_message>
Atualizando até agosto, sem contas da cidade
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -8,11 +8,11 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Curral do Fogo Velho CH" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Curral do Fogo Novo SI" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Sapecado 1" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Sapecado 2" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="Coqueiral" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="Curral do Fogo Velho CH" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Curral do Fogo Novo SI" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sapecado 1" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sapecado 2" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Coqueiral" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="49">
   <si>
     <t xml:space="preserve">Localidade</t>
   </si>
@@ -143,6 +143,21 @@
     <t xml:space="preserve">MAR/24</t>
   </si>
   <si>
+    <t xml:space="preserve">ABR/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAI/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JUN/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JUL/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGO/24</t>
+  </si>
+  <si>
     <t xml:space="preserve">Curral do Fogo Novo SI</t>
   </si>
   <si>
@@ -171,7 +186,7 @@
   <fonts count="6">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -227,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -267,6 +282,13 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -293,7 +315,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -342,8 +364,28 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -422,200 +464,31 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4f81bd"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="c0504d"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9bbb59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064a2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4bacc6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="f79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ff"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J1015"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="22.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="32.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="34.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="34.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="36.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="27.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="20.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="20.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1194,7 +1067,7 @@
       <c r="I18" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="J18" s="10" t="n">
+      <c r="J18" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1227,7 +1100,7 @@
       <c r="I19" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="J19" s="10" t="n">
+      <c r="J19" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1260,7 +1133,7 @@
       <c r="I20" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="J20" s="10" t="n">
+      <c r="J20" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1293,7 +1166,7 @@
       <c r="I21" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="J21" s="10" t="n">
+      <c r="J21" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1326,7 +1199,7 @@
       <c r="I22" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="J22" s="10" t="n">
+      <c r="J22" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1359,7 +1232,7 @@
       <c r="I23" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="J23" s="10" t="n">
+      <c r="J23" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1392,7 +1265,7 @@
       <c r="I24" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="J24" s="10" t="n">
+      <c r="J24" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1425,7 +1298,7 @@
       <c r="I25" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="J25" s="10" t="n">
+      <c r="J25" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1458,7 +1331,7 @@
       <c r="I26" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="J26" s="10" t="n">
+      <c r="J26" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1491,7 +1364,7 @@
       <c r="I27" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="J27" s="10" t="n">
+      <c r="J27" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1522,9 +1395,9 @@
         <v>3711.49</v>
       </c>
       <c r="I28" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="J28" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1535,70 +1408,220 @@
       <c r="B29" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="10" t="n">
+      <c r="C29" s="12" t="n">
         <v>655</v>
       </c>
-      <c r="D29" s="11" t="n">
+      <c r="D29" s="13" t="n">
         <v>23.39</v>
       </c>
-      <c r="E29" s="10" t="n">
+      <c r="E29" s="12" t="n">
         <v>28</v>
       </c>
-      <c r="F29" s="11" t="n">
+      <c r="F29" s="13" t="n">
         <f aca="false">H29-H28+G29</f>
         <v>376.97</v>
       </c>
-      <c r="G29" s="10" t="n">
+      <c r="G29" s="12" t="n">
         <v>605</v>
       </c>
-      <c r="H29" s="11" t="n">
+      <c r="H29" s="13" t="n">
         <v>3483.46</v>
       </c>
       <c r="I29" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J29" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="J29" s="13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12"/>
+      <c r="A30" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="14" t="n">
+        <v>32</v>
+      </c>
+      <c r="F30" s="13" t="n">
+        <f aca="false">H30-H29+G30</f>
+        <v>342.7</v>
+      </c>
+      <c r="G30" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="15" t="n">
+        <v>3826.16</v>
+      </c>
+      <c r="I30" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12"/>
+      <c r="A31" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="14" t="n">
+        <v>585</v>
+      </c>
+      <c r="D31" s="15" t="n">
+        <v>20.89</v>
+      </c>
+      <c r="E31" s="14" t="n">
+        <v>28</v>
+      </c>
+      <c r="F31" s="13" t="n">
+        <f aca="false">H31-H30+G31</f>
+        <v>379.5</v>
+      </c>
+      <c r="G31" s="14" t="n">
+        <v>535</v>
+      </c>
+      <c r="H31" s="15" t="n">
+        <v>3670.66</v>
+      </c>
+      <c r="I31" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="J31" s="15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12"/>
+      <c r="A32" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="14" t="n">
+        <v>553</v>
+      </c>
+      <c r="D32" s="15" t="n">
+        <v>17.28</v>
+      </c>
+      <c r="E32" s="14" t="n">
+        <v>32</v>
+      </c>
+      <c r="F32" s="13" t="n">
+        <f aca="false">H32-H31+G32</f>
+        <v>858</v>
+      </c>
+      <c r="G32" s="14" t="n">
+        <v>503</v>
+      </c>
+      <c r="H32" s="15" t="n">
+        <v>4025.66</v>
+      </c>
+      <c r="I32" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="J32" s="15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12"/>
+      <c r="A33" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="14" t="n">
+        <v>229</v>
+      </c>
+      <c r="D33" s="15" t="n">
+        <v>7.15</v>
+      </c>
+      <c r="E33" s="14" t="n">
+        <v>32</v>
+      </c>
+      <c r="F33" s="13" t="n">
+        <f aca="false">H33-H32+G33</f>
+        <v>691.6</v>
+      </c>
+      <c r="G33" s="14" t="n">
+        <v>179</v>
+      </c>
+      <c r="H33" s="15" t="n">
+        <v>4538.26</v>
+      </c>
+      <c r="I33" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="J33" s="15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12"/>
+      <c r="A34" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="14" t="n">
+        <v>502</v>
+      </c>
+      <c r="D34" s="15" t="n">
+        <v>16.19</v>
+      </c>
+      <c r="E34" s="14" t="n">
+        <v>31</v>
+      </c>
+      <c r="F34" s="13" t="n">
+        <f aca="false">H34-H33+G34</f>
+        <v>774.8</v>
+      </c>
+      <c r="G34" s="14" t="n">
+        <v>452</v>
+      </c>
+      <c r="H34" s="15" t="n">
+        <v>4861.06</v>
+      </c>
+      <c r="I34" s="14" t="n">
+        <v>50</v>
+      </c>
+      <c r="J34" s="15" t="n">
+        <v>50.72</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12"/>
+      <c r="A35" s="16"/>
     </row>
     <row r="36" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12"/>
+      <c r="A36" s="16"/>
     </row>
     <row r="37" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12"/>
+      <c r="A37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12"/>
+      <c r="A38" s="16"/>
     </row>
     <row r="39" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="12"/>
+      <c r="A39" s="16"/>
     </row>
     <row r="40" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12"/>
+      <c r="A40" s="16"/>
     </row>
     <row r="41" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12"/>
+      <c r="A41" s="16"/>
     </row>
     <row r="42" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12"/>
+      <c r="A42" s="16"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2575,7 +2598,7 @@
     <row r="1015" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -2585,28 +2608,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J1015"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="22.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="32.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="34.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="34.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="36.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="27.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="20.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="20.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2643,7 +2668,7 @@
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>11</v>
@@ -2675,7 +2700,7 @@
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>12</v>
@@ -2707,7 +2732,7 @@
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>13</v>
@@ -2739,7 +2764,7 @@
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>14</v>
@@ -2771,7 +2796,7 @@
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>15</v>
@@ -2803,7 +2828,7 @@
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>16</v>
@@ -2835,7 +2860,7 @@
     </row>
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>17</v>
@@ -2867,7 +2892,7 @@
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>18</v>
@@ -2899,7 +2924,7 @@
     </row>
     <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>19</v>
@@ -2931,7 +2956,7 @@
     </row>
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>20</v>
@@ -2963,7 +2988,7 @@
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>21</v>
@@ -2995,7 +3020,7 @@
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>22</v>
@@ -3027,7 +3052,7 @@
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>23</v>
@@ -3059,7 +3084,7 @@
     </row>
     <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>24</v>
@@ -3092,7 +3117,7 @@
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>25</v>
@@ -3125,7 +3150,7 @@
     </row>
     <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>26</v>
@@ -3158,7 +3183,7 @@
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>27</v>
@@ -3191,7 +3216,7 @@
     </row>
     <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>28</v>
@@ -3224,7 +3249,7 @@
     </row>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>29</v>
@@ -3257,7 +3282,7 @@
     </row>
     <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>30</v>
@@ -3290,7 +3315,7 @@
     </row>
     <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>31</v>
@@ -3323,7 +3348,7 @@
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>32</v>
@@ -3356,7 +3381,7 @@
     </row>
     <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>33</v>
@@ -3389,7 +3414,7 @@
     </row>
     <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>34</v>
@@ -3422,7 +3447,7 @@
     </row>
     <row r="26" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>35</v>
@@ -3455,7 +3480,7 @@
     </row>
     <row r="27" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>36</v>
@@ -3488,7 +3513,7 @@
     </row>
     <row r="28" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>37</v>
@@ -3521,77 +3546,231 @@
     </row>
     <row r="29" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="10" t="n">
+      <c r="C29" s="12" t="n">
         <v>720</v>
       </c>
-      <c r="D29" s="11" t="n">
+      <c r="D29" s="13" t="n">
         <v>25.71</v>
       </c>
-      <c r="E29" s="10" t="n">
+      <c r="E29" s="12" t="n">
         <v>28</v>
       </c>
-      <c r="F29" s="10" t="n">
+      <c r="F29" s="12" t="n">
         <f aca="false">H29-H28+G29</f>
         <v>1245.64</v>
       </c>
-      <c r="G29" s="10" t="n">
+      <c r="G29" s="12" t="n">
         <v>670</v>
       </c>
-      <c r="H29" s="11" t="n">
+      <c r="H29" s="13" t="n">
         <v>3553.92</v>
       </c>
-      <c r="I29" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J29" s="11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="I29" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="14" t="n">
+        <v>32</v>
+      </c>
+      <c r="F30" s="12" t="n">
+        <f aca="false">H30-H29+G30</f>
+        <v>2322.4</v>
+      </c>
+      <c r="G30" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="14" t="n">
+        <v>5876.32</v>
+      </c>
+      <c r="I30" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="14" t="n">
+        <v>640</v>
+      </c>
+      <c r="D31" s="15" t="n">
+        <v>22.85</v>
+      </c>
+      <c r="E31" s="14" t="n">
+        <v>28</v>
+      </c>
+      <c r="F31" s="12" t="n">
+        <f aca="false">H31-H30+G31</f>
+        <v>1254</v>
+      </c>
+      <c r="G31" s="14" t="n">
+        <v>590</v>
+      </c>
+      <c r="H31" s="14" t="n">
+        <v>6540.32</v>
+      </c>
+      <c r="I31" s="14" t="n">
+        <v>50</v>
+      </c>
+      <c r="J31" s="15" t="n">
+        <v>0</v>
+      </c>
+    </row>
     <row r="32" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12"/>
+      <c r="A32" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="14" t="n">
+        <v>640</v>
+      </c>
+      <c r="D32" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="E32" s="14" t="n">
+        <v>32</v>
+      </c>
+      <c r="F32" s="12" t="n">
+        <f aca="false">H32-H31+G32</f>
+        <v>706.200000000001</v>
+      </c>
+      <c r="G32" s="14" t="n">
+        <v>590</v>
+      </c>
+      <c r="H32" s="14" t="n">
+        <v>6656.52</v>
+      </c>
+      <c r="I32" s="14" t="n">
+        <v>50</v>
+      </c>
+      <c r="J32" s="15" t="n">
+        <v>14.27</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12"/>
+      <c r="A33" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="14" t="n">
+        <v>32</v>
+      </c>
+      <c r="F33" s="12" t="n">
+        <f aca="false">H33-H32+G33</f>
+        <v>569.24</v>
+      </c>
+      <c r="G33" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="14" t="n">
+        <v>7225.76</v>
+      </c>
+      <c r="I33" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="15" t="n">
+        <v>42.67</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12"/>
+      <c r="A34" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="14" t="n">
+        <v>440</v>
+      </c>
+      <c r="D34" s="15" t="n">
+        <v>14.19</v>
+      </c>
+      <c r="E34" s="14" t="n">
+        <v>31</v>
+      </c>
+      <c r="F34" s="12" t="n">
+        <f aca="false">H34-H33+G34</f>
+        <v>637.719999999999</v>
+      </c>
+      <c r="G34" s="14" t="n">
+        <v>390</v>
+      </c>
+      <c r="H34" s="14" t="n">
+        <v>7473.48</v>
+      </c>
+      <c r="I34" s="14" t="n">
+        <v>50</v>
+      </c>
+      <c r="J34" s="15" t="n">
+        <v>50.78</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12"/>
+      <c r="A35" s="16"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12"/>
+      <c r="A36" s="16"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12"/>
+      <c r="A37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12"/>
+      <c r="A38" s="16"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="12"/>
+      <c r="A39" s="16"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12"/>
+      <c r="A40" s="16"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12"/>
+      <c r="A41" s="16"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12"/>
+      <c r="A42" s="16"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="12"/>
+      <c r="A43" s="16"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="12"/>
+      <c r="A44" s="16"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4566,7 +4745,7 @@
     <row r="1015" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -4576,29 +4755,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:K1015"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K30" activeCellId="0" sqref="K30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="22.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="27.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="32.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="34.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="34.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="36.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="27.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="20.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="20.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4618,7 +4799,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>5</v>
@@ -4638,7 +4819,7 @@
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>11</v>
@@ -4673,7 +4854,7 @@
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>12</v>
@@ -4708,7 +4889,7 @@
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>13</v>
@@ -4743,7 +4924,7 @@
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>14</v>
@@ -4778,7 +4959,7 @@
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>15</v>
@@ -4813,7 +4994,7 @@
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>16</v>
@@ -4848,7 +5029,7 @@
     </row>
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>17</v>
@@ -4883,7 +5064,7 @@
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>18</v>
@@ -4918,7 +5099,7 @@
     </row>
     <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>19</v>
@@ -4953,7 +5134,7 @@
     </row>
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>20</v>
@@ -4988,7 +5169,7 @@
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>21</v>
@@ -5023,7 +5204,7 @@
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>22</v>
@@ -5058,7 +5239,7 @@
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>23</v>
@@ -5093,7 +5274,7 @@
     </row>
     <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>24</v>
@@ -5129,7 +5310,7 @@
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>25</v>
@@ -5165,7 +5346,7 @@
     </row>
     <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>26</v>
@@ -5201,7 +5382,7 @@
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>27</v>
@@ -5237,7 +5418,7 @@
     </row>
     <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>28</v>
@@ -5273,7 +5454,7 @@
     </row>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>29</v>
@@ -5309,7 +5490,7 @@
     </row>
     <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>30</v>
@@ -5345,7 +5526,7 @@
     </row>
     <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>31</v>
@@ -5381,7 +5562,7 @@
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>32</v>
@@ -5417,7 +5598,7 @@
     </row>
     <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>33</v>
@@ -5453,7 +5634,7 @@
     </row>
     <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>34</v>
@@ -5489,7 +5670,7 @@
     </row>
     <row r="26" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>35</v>
@@ -5525,7 +5706,7 @@
     </row>
     <row r="27" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>36</v>
@@ -5561,7 +5742,7 @@
     </row>
     <row r="28" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>37</v>
@@ -5597,80 +5778,247 @@
     </row>
     <row r="29" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="10" t="n">
+      <c r="C29" s="12" t="n">
         <v>242</v>
       </c>
-      <c r="D29" s="11" t="n">
+      <c r="D29" s="13" t="n">
         <v>8.34</v>
       </c>
-      <c r="E29" s="10" t="n">
+      <c r="E29" s="12" t="n">
         <v>29</v>
       </c>
-      <c r="F29" s="10" t="n">
+      <c r="F29" s="12" t="n">
         <f aca="false">1040+791</f>
         <v>1831</v>
       </c>
-      <c r="G29" s="10" t="n">
+      <c r="G29" s="12" t="n">
         <f aca="false">I29-I28+H29</f>
         <v>192</v>
       </c>
-      <c r="H29" s="10" t="n">
+      <c r="H29" s="12" t="n">
         <v>192</v>
       </c>
-      <c r="I29" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J29" s="10" t="n">
+      <c r="I29" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="12" t="n">
         <v>50</v>
       </c>
-      <c r="K29" s="11" t="n">
+      <c r="K29" s="13" t="n">
         <v>47.92</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="14" t="n">
+        <v>320</v>
+      </c>
+      <c r="D30" s="15" t="n">
+        <v>10.32</v>
+      </c>
+      <c r="E30" s="14" t="n">
+        <v>31</v>
+      </c>
+      <c r="F30" s="14" t="n">
+        <v>1760</v>
+      </c>
+      <c r="G30" s="12" t="n">
+        <f aca="false">I30-I29+H30</f>
+        <v>270</v>
+      </c>
+      <c r="H30" s="14" t="n">
+        <v>270</v>
+      </c>
+      <c r="I30" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="14" t="n">
+        <v>50</v>
+      </c>
+      <c r="K30" s="15" t="n">
+        <v>47.75</v>
+      </c>
+    </row>
     <row r="31" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12"/>
+      <c r="A31" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="14" t="n">
+        <v>320</v>
+      </c>
+      <c r="D31" s="15" t="n">
+        <v>11.03</v>
+      </c>
+      <c r="E31" s="14" t="n">
+        <v>29</v>
+      </c>
+      <c r="F31" s="14" t="n">
+        <v>1920</v>
+      </c>
+      <c r="G31" s="12" t="n">
+        <f aca="false">I31-I30+H31</f>
+        <v>270</v>
+      </c>
+      <c r="H31" s="14" t="n">
+        <v>270</v>
+      </c>
+      <c r="I31" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="14" t="n">
+        <v>50</v>
+      </c>
+      <c r="K31" s="15" t="n">
+        <v>47.92</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12"/>
+      <c r="A32" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="14" t="n">
+        <v>320</v>
+      </c>
+      <c r="D32" s="15" t="n">
+        <v>9.69</v>
+      </c>
+      <c r="E32" s="14" t="n">
+        <v>33</v>
+      </c>
+      <c r="F32" s="14" t="n">
+        <v>1920</v>
+      </c>
+      <c r="G32" s="12" t="n">
+        <f aca="false">I32-I31+H32</f>
+        <v>270</v>
+      </c>
+      <c r="H32" s="14" t="n">
+        <v>270</v>
+      </c>
+      <c r="I32" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="14" t="n">
+        <v>50</v>
+      </c>
+      <c r="K32" s="15" t="n">
+        <v>50.54</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12"/>
+      <c r="A33" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="14" t="n">
+        <v>360</v>
+      </c>
+      <c r="D33" s="15" t="n">
+        <v>12</v>
+      </c>
+      <c r="E33" s="14" t="n">
+        <v>30</v>
+      </c>
+      <c r="F33" s="14" t="n">
+        <v>1640</v>
+      </c>
+      <c r="G33" s="12" t="n">
+        <f aca="false">I33-I32+H33</f>
+        <v>310</v>
+      </c>
+      <c r="H33" s="14" t="n">
+        <v>310</v>
+      </c>
+      <c r="I33" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="14" t="n">
+        <v>50</v>
+      </c>
+      <c r="K33" s="15" t="n">
+        <v>51.86</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12"/>
+      <c r="A34" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="14" t="n">
+        <v>360</v>
+      </c>
+      <c r="D34" s="15" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="E34" s="14" t="n">
+        <v>33</v>
+      </c>
+      <c r="F34" s="14" t="n">
+        <v>1800</v>
+      </c>
+      <c r="G34" s="12" t="n">
+        <f aca="false">I34-I33+H34</f>
+        <v>310</v>
+      </c>
+      <c r="H34" s="14" t="n">
+        <v>310</v>
+      </c>
+      <c r="I34" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="14" t="n">
+        <v>50</v>
+      </c>
+      <c r="K34" s="15" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12"/>
+      <c r="A35" s="16"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12"/>
+      <c r="A36" s="16"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12"/>
+      <c r="A37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12"/>
+      <c r="A38" s="16"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="12"/>
+      <c r="A39" s="16"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12"/>
+      <c r="A40" s="16"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12"/>
+      <c r="A41" s="16"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12"/>
+      <c r="A42" s="16"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="12"/>
+      <c r="A43" s="16"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6646,7 +6994,7 @@
     <row r="1015" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -6656,28 +7004,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J1015"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J29" activeCellId="0" sqref="J29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="22.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="32.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="34.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="34.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="36.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="27.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="20.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="20.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6714,7 +7064,7 @@
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>11</v>
@@ -6746,7 +7096,7 @@
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>12</v>
@@ -6778,7 +7128,7 @@
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>13</v>
@@ -6810,7 +7160,7 @@
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>14</v>
@@ -6842,7 +7192,7 @@
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>15</v>
@@ -6874,7 +7224,7 @@
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>16</v>
@@ -6906,7 +7256,7 @@
     </row>
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>17</v>
@@ -6938,7 +7288,7 @@
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>18</v>
@@ -6970,7 +7320,7 @@
     </row>
     <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>19</v>
@@ -7002,7 +7352,7 @@
     </row>
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>20</v>
@@ -7034,7 +7384,7 @@
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>21</v>
@@ -7066,7 +7416,7 @@
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>22</v>
@@ -7098,7 +7448,7 @@
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>23</v>
@@ -7130,7 +7480,7 @@
     </row>
     <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>24</v>
@@ -7163,7 +7513,7 @@
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>25</v>
@@ -7196,7 +7546,7 @@
     </row>
     <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>26</v>
@@ -7229,7 +7579,7 @@
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>27</v>
@@ -7262,7 +7612,7 @@
     </row>
     <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>28</v>
@@ -7295,7 +7645,7 @@
     </row>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>29</v>
@@ -7328,7 +7678,7 @@
     </row>
     <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>30</v>
@@ -7361,7 +7711,7 @@
     </row>
     <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>31</v>
@@ -7394,7 +7744,7 @@
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>32</v>
@@ -7427,7 +7777,7 @@
     </row>
     <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>33</v>
@@ -7460,7 +7810,7 @@
     </row>
     <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>34</v>
@@ -7493,7 +7843,7 @@
     </row>
     <row r="26" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>35</v>
@@ -7526,7 +7876,7 @@
     </row>
     <row r="27" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>36</v>
@@ -7559,7 +7909,7 @@
     </row>
     <row r="28" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>37</v>
@@ -7592,7 +7942,7 @@
     </row>
     <row r="29" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>38</v>
@@ -7604,7 +7954,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="10" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F29" s="11" t="n">
         <f aca="false">H29-H28+G29</f>
@@ -7623,45 +7973,197 @@
         <v>23.57</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="14" t="n">
+        <v>30</v>
+      </c>
+      <c r="F30" s="11" t="n">
+        <f aca="false">H30-H29+G30</f>
+        <v>7.44999999999999</v>
+      </c>
+      <c r="G30" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="15" t="n">
+        <v>392.68</v>
+      </c>
+      <c r="I30" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="15" t="n">
+        <v>23.5</v>
+      </c>
+    </row>
     <row r="31" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12"/>
+      <c r="A31" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="14" t="n">
+        <v>29</v>
+      </c>
+      <c r="F31" s="11" t="n">
+        <f aca="false">H31-H30+G31</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="15" t="n">
+        <v>392.68</v>
+      </c>
+      <c r="I31" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="15" t="n">
+        <v>23.57</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12"/>
+      <c r="A32" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="14" t="n">
+        <v>33</v>
+      </c>
+      <c r="F32" s="11" t="n">
+        <f aca="false">H32-H31+G32</f>
+        <v>8.25</v>
+      </c>
+      <c r="G32" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="15" t="n">
+        <v>400.93</v>
+      </c>
+      <c r="I32" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="15" t="n">
+        <v>24.86</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12"/>
+      <c r="A33" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="14" t="n">
+        <v>30</v>
+      </c>
+      <c r="F33" s="11" t="n">
+        <f aca="false">H33-H32+G33</f>
+        <v>3.30000000000001</v>
+      </c>
+      <c r="G33" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="15" t="n">
+        <v>404.23</v>
+      </c>
+      <c r="I33" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="15" t="n">
+        <v>25.52</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12"/>
+      <c r="A34" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="14" t="n">
+        <v>33</v>
+      </c>
+      <c r="F34" s="11" t="n">
+        <f aca="false">H34-H33+G34</f>
+        <v>2.65999999999997</v>
+      </c>
+      <c r="G34" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="15" t="n">
+        <v>406.89</v>
+      </c>
+      <c r="I34" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="15" t="n">
+        <v>25.09</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12"/>
+      <c r="A35" s="16"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12"/>
+      <c r="A36" s="16"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12"/>
+      <c r="A37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12"/>
+      <c r="A38" s="16"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="12"/>
+      <c r="A39" s="16"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12"/>
+      <c r="A40" s="16"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12"/>
+      <c r="A41" s="16"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12"/>
+      <c r="A42" s="16"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="12"/>
+      <c r="A43" s="16"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -8637,7 +9139,7 @@
     <row r="1015" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -8647,28 +9149,30 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J1015"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="22.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="32.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="34.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="34.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="36.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="27.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="20.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="20.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8705,7 +9209,7 @@
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>11</v>
@@ -8737,7 +9241,7 @@
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>12</v>
@@ -8769,7 +9273,7 @@
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>13</v>
@@ -8801,9 +9305,9 @@
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="10" t="n">
@@ -8833,7 +9337,7 @@
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>15</v>
@@ -8865,7 +9369,7 @@
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>16</v>
@@ -8897,7 +9401,7 @@
     </row>
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>17</v>
@@ -8929,7 +9433,7 @@
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>18</v>
@@ -8961,7 +9465,7 @@
     </row>
     <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>19</v>
@@ -8993,7 +9497,7 @@
     </row>
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>20</v>
@@ -9025,7 +9529,7 @@
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>21</v>
@@ -9057,7 +9561,7 @@
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>22</v>
@@ -9089,7 +9593,7 @@
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>23</v>
@@ -9121,7 +9625,7 @@
     </row>
     <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>24</v>
@@ -9154,7 +9658,7 @@
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>25</v>
@@ -9187,7 +9691,7 @@
     </row>
     <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>26</v>
@@ -9220,7 +9724,7 @@
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>27</v>
@@ -9253,7 +9757,7 @@
     </row>
     <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>28</v>
@@ -9286,7 +9790,7 @@
     </row>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>29</v>
@@ -9319,7 +9823,7 @@
     </row>
     <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>30</v>
@@ -9352,7 +9856,7 @@
     </row>
     <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>31</v>
@@ -9385,7 +9889,7 @@
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>32</v>
@@ -9418,7 +9922,7 @@
     </row>
     <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>33</v>
@@ -9451,7 +9955,7 @@
     </row>
     <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>34</v>
@@ -9484,7 +9988,7 @@
     </row>
     <row r="26" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>35</v>
@@ -9517,7 +10021,7 @@
     </row>
     <row r="27" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>36</v>
@@ -9550,7 +10054,7 @@
     </row>
     <row r="28" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>37</v>
@@ -9583,7 +10087,7 @@
     </row>
     <row r="29" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>38</v>
@@ -9614,45 +10118,112 @@
         <v>60.27</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="15"/>
+    </row>
     <row r="31" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12"/>
+      <c r="A31" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="15"/>
     </row>
     <row r="32" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12"/>
+      <c r="A32" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="15"/>
     </row>
     <row r="33" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12"/>
+      <c r="A33" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="15"/>
     </row>
     <row r="34" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12"/>
+      <c r="A34" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="15"/>
     </row>
     <row r="35" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12"/>
+      <c r="A35" s="16"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12"/>
+      <c r="A36" s="16"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12"/>
+      <c r="A37" s="16"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12"/>
+      <c r="A38" s="16"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="12"/>
+      <c r="A39" s="16"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12"/>
+      <c r="A40" s="16"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12"/>
+      <c r="A41" s="16"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12"/>
+      <c r="A42" s="16"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="12"/>
+      <c r="A43" s="16"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -10628,7 +11199,7 @@
     <row r="1015" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>